<commit_message>
retrive vehicle functionality implementation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,26 @@
           <t>wheels</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>stageId</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>stageName</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>slot</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>datetime</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,13 +506,123 @@
           <t>data@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
+      <c r="E2" t="n">
+        <v>1234567890</v>
       </c>
       <c r="F2" t="n">
         <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Slot 1</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-01-29 20:23:18.351679</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Slot 1</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025-01-29 20:25:44.348060</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Slot 2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2025-01-29 20:26:03.309266</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>